<commit_message>
todo el pdf andaaaa agregue anexo
</commit_message>
<xml_diff>
--- a/ej 1/prueba.xlsx
+++ b/ej 1/prueba.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\ITBA\7° Cuatrimestre\Teoría de Circuitos\Trabajos Prácticos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rochi\Google Drive\Materias\Teoría de circuitos\TPs\TP1\TC_TP1\ej 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BF0BCFA6-7C85-42F2-8777-24E5BBE524EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20493" windowHeight="6933" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,7 +71,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,7 +131,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -423,22 +426,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E2" sqref="E2:E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.41015625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13.41015625" customWidth="1"/>
-    <col min="5" max="5" width="14.41015625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -471,7 +474,7 @@
       <c r="D2">
         <v>-22</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f>20*LOG(C2/B2)</f>
         <v>-0.53989728915165058</v>
       </c>
@@ -480,7 +483,7 @@
         <v>0.93973442288049036</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -493,16 +496,16 @@
       <c r="D3">
         <v>-37</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E41" si="0">20*LOG(C3/B3)</f>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E35" si="0">20*LOG(C3/B3)</f>
         <v>-2.1189214744849276</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H42" si="1">C3/B3</f>
+        <f t="shared" ref="H3:H35" si="1">C3/B3</f>
         <v>0.7835269271383315</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -515,7 +518,7 @@
       <c r="D4">
         <v>-50</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>-3.9569356616889895</v>
       </c>
@@ -524,7 +527,7 @@
         <v>0.63409337676438648</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -537,7 +540,7 @@
       <c r="D5">
         <v>-60</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>-5.9917909660134772</v>
       </c>
@@ -546,7 +549,7 @@
         <v>0.50166112956810638</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -559,7 +562,7 @@
       <c r="D6">
         <v>-67</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>-8.241172179272013</v>
       </c>
@@ -568,7 +571,7 @@
         <v>0.38720538720538722</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -581,7 +584,7 @@
       <c r="D7">
         <v>-72</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>-10.566708021475339</v>
       </c>
@@ -590,7 +593,7 @@
         <v>0.2962542565266742</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -603,7 +606,7 @@
       <c r="D8">
         <v>-78</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>-13.217899120105987</v>
       </c>
@@ -612,7 +615,7 @@
         <v>0.21832579185520362</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -625,7 +628,7 @@
       <c r="D9">
         <v>-82</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>-16.448513243203813</v>
       </c>
@@ -634,7 +637,7 @@
         <v>0.15051311288483468</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -647,7 +650,7 @@
       <c r="D10">
         <v>-84</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>-20.878977391884366</v>
       </c>
@@ -656,7 +659,7 @@
         <v>9.0375586854460094E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9.5</v>
       </c>
@@ -669,7 +672,7 @@
       <c r="D11">
         <v>-85</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>-23.750414416729264</v>
       </c>
@@ -678,7 +681,7 @@
         <v>6.4935064935064929E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -691,7 +694,7 @@
       <c r="D12">
         <v>-86</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>-28.238513097776252</v>
       </c>
@@ -700,7 +703,7 @@
         <v>3.8732394366197187E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10.199999999999999</v>
       </c>
@@ -713,7 +716,7 @@
       <c r="D13">
         <v>-87</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>-30.639791028251008</v>
       </c>
@@ -722,7 +725,7 @@
         <v>2.9377203290246769E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10.4</v>
       </c>
@@ -735,7 +738,7 @@
       <c r="D14">
         <v>-88</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <f t="shared" si="0"/>
         <v>-33.969175377313576</v>
       </c>
@@ -744,7 +747,7 @@
         <v>2.0023557126030624E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10.6</v>
       </c>
@@ -757,7 +760,7 @@
       <c r="D15">
         <v>-89</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
         <v>-39.729327180347084</v>
       </c>
@@ -766,7 +769,7 @@
         <v>1.0316529894490035E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10.8</v>
       </c>
@@ -779,14 +782,14 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>-50</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -799,7 +802,7 @@
       <c r="D17">
         <v>88</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>-40.618063536785975</v>
       </c>
@@ -808,7 +811,7 @@
         <v>9.3131548311990685E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11.2</v>
       </c>
@@ -821,7 +824,7 @@
       <c r="D18">
         <v>87</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>-34.986034660272871</v>
       </c>
@@ -830,7 +833,7 @@
         <v>1.781140861466822E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11.4</v>
       </c>
@@ -843,7 +846,7 @@
       <c r="D19">
         <v>88</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>-31.055391604231843</v>
       </c>
@@ -852,7 +855,7 @@
         <v>2.8004667444574093E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11.6</v>
       </c>
@@ -865,7 +868,7 @@
       <c r="D20">
         <v>88</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>-28.812088417877998</v>
       </c>
@@ -874,7 +877,7 @@
         <v>3.6257309941520467E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11.8</v>
       </c>
@@ -887,7 +890,7 @@
       <c r="D21">
         <v>86</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>-26.899577305163991</v>
       </c>
@@ -896,7 +899,7 @@
         <v>4.5187793427230047E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -909,7 +912,7 @@
       <c r="D22">
         <v>87</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>-25.476627161435118</v>
       </c>
@@ -918,7 +921,7 @@
         <v>5.3231492361927146E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>13</v>
       </c>
@@ -931,7 +934,7 @@
       <c r="D23">
         <v>84</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>-20.605126380805313</v>
       </c>
@@ -940,7 +943,7 @@
         <v>9.3270365997638716E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14</v>
       </c>
@@ -953,7 +956,7 @@
       <c r="D24">
         <v>83</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>-17.668066212793743</v>
       </c>
@@ -962,7 +965,7 @@
         <v>0.13079667063020214</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>15</v>
       </c>
@@ -975,7 +978,7 @@
       <c r="D25">
         <v>78</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>-15.699318166543906</v>
       </c>
@@ -984,7 +987,7 @@
         <v>0.16407185628742518</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>16</v>
       </c>
@@ -997,7 +1000,7 @@
       <c r="D26">
         <v>78</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>-14.084684886567523</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>0.1975903614457831</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>17</v>
       </c>
@@ -1019,7 +1022,7 @@
       <c r="D27">
         <v>76</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <f t="shared" si="0"/>
         <v>-12.754006951941923</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>0.23030303030303029</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>18</v>
       </c>
@@ -1041,7 +1044,7 @@
       <c r="D28">
         <v>75</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <f t="shared" si="0"/>
         <v>-11.831891152995947</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>0.25609756097560976</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>19</v>
       </c>
@@ -1063,7 +1066,7 @@
       <c r="D29">
         <v>73</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <f t="shared" si="0"/>
         <v>-10.977931377432169</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>0.28255528255528251</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20</v>
       </c>
@@ -1085,7 +1088,7 @@
       <c r="D30">
         <v>72</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <f t="shared" si="0"/>
         <v>-10.210900204132242</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>0.30864197530864201</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>25</v>
       </c>
@@ -1107,7 +1110,7 @@
       <c r="D31">
         <v>65</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <f t="shared" si="0"/>
         <v>-7.4716132562518585</v>
       </c>
@@ -1116,7 +1119,7 @@
         <v>0.42307692307692307</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1129,7 +1132,7 @@
       <c r="D32">
         <v>58</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <f t="shared" si="0"/>
         <v>-5.9647419095962224</v>
       </c>
@@ -1138,7 +1141,7 @@
         <v>0.50322580645161286</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>35</v>
       </c>
@@ -1151,7 +1154,7 @@
       <c r="D33">
         <v>54</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <f t="shared" si="0"/>
         <v>-4.6321717381102525</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>0.58666666666666667</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>40</v>
       </c>
@@ -1173,7 +1176,7 @@
       <c r="D34">
         <v>50</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <f t="shared" si="0"/>
         <v>-3.8245000436947683</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>0.64383561643835618</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>50</v>
       </c>
@@ -1195,7 +1198,7 @@
       <c r="D35">
         <v>42</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <f t="shared" si="0"/>
         <v>-2.7051001016855225</v>
       </c>

</xml_diff>